<commit_message>
Enhance daily stock management
</commit_message>
<xml_diff>
--- a/public/file/format-import-Forecast(system-sto).xlsx
+++ b/public/file/format-import-Forecast(system-sto).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\system-sto-kbi\public\file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A907AFC-D5BE-48D5-BFEF-34EBBDBB50B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BCB3BEE-1888-4CCF-8C02-EC808136AD0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{235D7ECB-1AB5-47C9-9C87-335BE7A2122F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>part_number</t>
   </si>
@@ -46,9 +46,6 @@
   </si>
   <si>
     <t>part_name</t>
-  </si>
-  <si>
-    <t>qty_box</t>
   </si>
   <si>
     <t>forecast_month</t>
@@ -448,10 +445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4B65D39-E4F5-41EC-A577-54771F0AEB14}">
-  <dimension ref="A1:I33"/>
+  <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="D10" activeCellId="1" sqref="D1 A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -459,13 +456,12 @@
     <col min="1" max="1" width="23.81640625" customWidth="1"/>
     <col min="2" max="2" width="25.26953125" customWidth="1"/>
     <col min="3" max="3" width="26.26953125" customWidth="1"/>
-    <col min="4" max="4" width="22.6328125" customWidth="1"/>
-    <col min="5" max="5" width="25.90625" customWidth="1"/>
-    <col min="6" max="6" width="20.08984375" customWidth="1"/>
-    <col min="7" max="7" width="23.26953125" customWidth="1"/>
+    <col min="4" max="4" width="25.90625" customWidth="1"/>
+    <col min="5" max="5" width="20.08984375" customWidth="1"/>
+    <col min="6" max="6" width="23.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -476,309 +472,274 @@
         <v>0</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>6</v>
-      </c>
+      <c r="G1" s="1"/>
       <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
+      <c r="G2" s="2"/>
       <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="5"/>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="5"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="5"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
-      <c r="G27" s="5"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="5"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
-      <c r="G28" s="5"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" s="5"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
       <c r="E30" s="5"/>
       <c r="F30" s="5"/>
-      <c r="G30" s="5"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" s="5"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
       <c r="E31" s="5"/>
       <c r="F31" s="5"/>
-      <c r="G31" s="5"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" s="5"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
-      <c r="G32" s="5"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" s="5"/>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
       <c r="E33" s="5"/>
       <c r="F33" s="5"/>
-      <c r="G33" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix: improve duplicate part logging and enhance UI for various import templates
</commit_message>
<xml_diff>
--- a/public/file/format-import-Forecast(system-sto).xlsx
+++ b/public/file/format-import-Forecast(system-sto).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\system-sto-kbi\public\file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BCB3BEE-1888-4CCF-8C02-EC808136AD0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6E76CA4-C4E4-4EFD-A663-5EE6C133F872}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{235D7ECB-1AB5-47C9-9C87-335BE7A2122F}"/>
   </bookViews>
@@ -130,7 +130,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -448,7 +448,7 @@
   <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" activeCellId="1" sqref="D1 A1:XFD1048576"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Refactor views, update forms, enhance reports, add modal, cleanup layout/routes.
</commit_message>
<xml_diff>
--- a/public/file/format-import-Forecast(system-sto).xlsx
+++ b/public/file/format-import-Forecast(system-sto).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\system-sto-kbi\public\file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6E76CA4-C4E4-4EFD-A663-5EE6C133F872}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A1C4D30-499D-4046-95B5-E615D5718204}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{235D7ECB-1AB5-47C9-9C87-335BE7A2122F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>part_number</t>
   </si>
@@ -52,6 +52,9 @@
   </si>
   <si>
     <t>po_pcs</t>
+  </si>
+  <si>
+    <t>Customer</t>
   </si>
 </sst>
 </file>
@@ -130,7 +133,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -445,10 +448,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4B65D39-E4F5-41EC-A577-54771F0AEB14}">
-  <dimension ref="A1:H33"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -472,274 +475,28 @@
         <v>0</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1"/>
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
+      <c r="D2" s="5"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
-      <c r="G2" s="2"/>
+      <c r="G2" s="4"/>
       <c r="H2" s="2"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A19" s="5"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A20" s="5"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A21" s="5"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A22" s="5"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A23" s="5"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A24" s="5"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A25" s="5"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A26" s="5"/>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A27" s="5"/>
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A28" s="5"/>
-      <c r="B28" s="5"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="5"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A29" s="5"/>
-      <c r="B29" s="5"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="5"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A30" s="5"/>
-      <c r="B30" s="5"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5"/>
-      <c r="F30" s="5"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A31" s="5"/>
-      <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="5"/>
-      <c r="F31" s="5"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A32" s="5"/>
-      <c r="B32" s="5"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="5"/>
-      <c r="F32" s="5"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A33" s="5"/>
-      <c r="B33" s="5"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="5"/>
-      <c r="E33" s="5"/>
-      <c r="F33" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>